<commit_message>
Fix code and update deployment
</commit_message>
<xml_diff>
--- a/中央値と下限値の推移.xlsx
+++ b/中央値と下限値の推移.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryusuke/Desktop/bitcoininvestment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91ECC5A3-D709-6040-9F0A-15C4F2FF925F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FFB24A-C148-3F4D-A456-2077A7BB64E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="6260" windowWidth="27500" windowHeight="16360" xr2:uid="{06519336-3EE9-2547-A8F6-1E3A42306076}"/>
+    <workbookView xWindow="2340" yWindow="19360" windowWidth="27500" windowHeight="16360" xr2:uid="{06519336-3EE9-2547-A8F6-1E3A42306076}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Days Since 2009-01-03</t>
-  </si>
-  <si>
     <t>中央値</t>
     <rPh sb="0" eb="3">
       <t xml:space="preserve">チュウオウチ </t>
@@ -57,15 +54,15 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-  </numFmts>
-  <fonts count="5">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -80,24 +77,6 @@
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <name val="MS Mincho"/>
-      <family val="2"/>
-      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,24 +101,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="26" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,394 +444,386 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04E2A05-8E87-2A42-8263-D4D277E99F75}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" style="5" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="31" defaultRowHeight="20"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="3">
+      <c r="A2">
         <v>2025</v>
       </c>
-      <c r="B2" s="3">
-        <v>5877</v>
-      </c>
-      <c r="C2" s="4">
-        <v>122688.51</v>
-      </c>
-      <c r="D2" s="4">
-        <v>22086.09</v>
+      <c r="B2" s="1">
+        <v>46022</v>
+      </c>
+      <c r="C2">
+        <v>142366.32910984699</v>
+      </c>
+      <c r="D2">
+        <v>64298.7538957461</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3">
+      <c r="A3">
         <v>2026</v>
       </c>
-      <c r="B3" s="3">
-        <v>6242</v>
-      </c>
-      <c r="C3" s="4">
-        <v>170941.9</v>
-      </c>
-      <c r="D3" s="4">
-        <v>32695.55</v>
+      <c r="B3" s="1">
+        <v>46387</v>
+      </c>
+      <c r="C3">
+        <v>198829.46175720601</v>
+      </c>
+      <c r="D3">
+        <v>90216.105349420599</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="3">
+      <c r="A4">
         <v>2027</v>
       </c>
-      <c r="B4" s="3">
-        <v>6607</v>
-      </c>
-      <c r="C4" s="4">
-        <v>237347.64</v>
-      </c>
-      <c r="D4" s="4">
-        <v>49020.95</v>
+      <c r="B4" s="1">
+        <v>46752</v>
+      </c>
+      <c r="C4">
+        <v>272715.36749770597</v>
+      </c>
+      <c r="D4">
+        <v>124283.20222362901</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="3">
+      <c r="A5">
         <v>2028</v>
       </c>
-      <c r="B5" s="3">
-        <v>6972</v>
-      </c>
-      <c r="C5" s="4">
-        <v>327853.92</v>
-      </c>
-      <c r="D5" s="4">
-        <v>73073.960000000006</v>
+      <c r="B5" s="1">
+        <v>47118</v>
+      </c>
+      <c r="C5">
+        <v>368338.05844702403</v>
+      </c>
+      <c r="D5">
+        <v>168560.68067913101</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="3">
+      <c r="A6">
         <v>2029</v>
       </c>
-      <c r="B6" s="3">
-        <v>7337</v>
-      </c>
-      <c r="C6" s="4">
-        <v>450782.62</v>
-      </c>
-      <c r="D6" s="4">
-        <v>107798.65</v>
+      <c r="B6" s="1">
+        <v>47483</v>
+      </c>
+      <c r="C6">
+        <v>489854.30059245299</v>
+      </c>
+      <c r="D6">
+        <v>225055.94793182999</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="3">
+      <c r="A7">
         <v>2030</v>
       </c>
-      <c r="B7" s="3">
-        <v>7702</v>
-      </c>
-      <c r="C7" s="4">
-        <v>618184.25</v>
-      </c>
-      <c r="D7" s="4">
-        <v>157328.99</v>
+      <c r="B7" s="1">
+        <v>47848</v>
+      </c>
+      <c r="C7">
+        <v>642876.44219960202</v>
+      </c>
+      <c r="D7">
+        <v>296473.06622865202</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="3">
+      <c r="A8">
         <v>2031</v>
       </c>
-      <c r="B8" s="3">
-        <v>8067</v>
-      </c>
-      <c r="C8" s="4">
-        <v>849285.83</v>
-      </c>
-      <c r="D8" s="4">
-        <v>225043.56</v>
+      <c r="B8" s="1">
+        <v>48213</v>
+      </c>
+      <c r="C8">
+        <v>833566.91976404004</v>
+      </c>
+      <c r="D8">
+        <v>385797.78668842802</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="3">
+      <c r="A9">
         <v>2032</v>
       </c>
-      <c r="B9" s="3">
-        <v>8432</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1156653.21</v>
-      </c>
-      <c r="D9" s="4">
-        <v>314793.99</v>
+      <c r="B9" s="1">
+        <v>48579</v>
+      </c>
+      <c r="C9">
+        <v>1069651.28559435</v>
+      </c>
+      <c r="D9">
+        <v>496775.94948903</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="3">
+      <c r="A10">
         <v>2033</v>
       </c>
-      <c r="B10" s="3">
-        <v>8797</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1565101.39</v>
-      </c>
-      <c r="D10" s="4">
-        <v>432265.78</v>
+      <c r="B10" s="1">
+        <v>48944</v>
+      </c>
+      <c r="C10">
+        <v>1357793.6097800201</v>
+      </c>
+      <c r="D10">
+        <v>632682.74721713201</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="3">
+      <c r="A11">
         <v>2034</v>
       </c>
-      <c r="B11" s="3">
-        <v>9162</v>
-      </c>
-      <c r="C11" s="4">
-        <v>2092721.04</v>
-      </c>
-      <c r="D11" s="4">
-        <v>583119.31000000006</v>
+      <c r="B11" s="1">
+        <v>49309</v>
+      </c>
+      <c r="C11">
+        <v>1707509.5331403699</v>
+      </c>
+      <c r="D11">
+        <v>798165.63930554595</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="3">
+      <c r="A12">
         <v>2035</v>
       </c>
-      <c r="B12" s="3">
-        <v>9527</v>
-      </c>
-      <c r="C12" s="4">
-        <v>2769254.89</v>
-      </c>
-      <c r="D12" s="4">
-        <v>773188.23</v>
+      <c r="B12" s="1">
+        <v>49674</v>
+      </c>
+      <c r="C12">
+        <v>2128810.2096995101</v>
+      </c>
+      <c r="D12">
+        <v>998142.41460257897</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="3">
+      <c r="A13">
         <v>2036</v>
       </c>
-      <c r="B13" s="3">
-        <v>9892</v>
-      </c>
-      <c r="C13" s="4">
-        <v>3627039.89</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1010507.88</v>
+      <c r="B13" s="1">
+        <v>50040</v>
+      </c>
+      <c r="C13">
+        <v>2634369.1179597699</v>
+      </c>
+      <c r="D13">
+        <v>1238833.9615905201</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="3">
+      <c r="A14">
         <v>2037</v>
       </c>
-      <c r="B14" s="3">
-        <v>10257</v>
-      </c>
-      <c r="C14" s="4">
-        <v>4711068.1100000003</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1304553.31</v>
+      <c r="B14" s="1">
+        <v>50405</v>
+      </c>
+      <c r="C14">
+        <v>3233861.4796145102</v>
+      </c>
+      <c r="D14">
+        <v>1525072.26709835</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="3">
+      <c r="A15">
         <v>2038</v>
       </c>
-      <c r="B15" s="3">
-        <v>10622</v>
-      </c>
-      <c r="C15" s="4">
-        <v>6069440.4800000004</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1666419.28</v>
+      <c r="B15" s="1">
+        <v>50770</v>
+      </c>
+      <c r="C15">
+        <v>3942287.2525885501</v>
+      </c>
+      <c r="D15">
+        <v>1864266.6780311801</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="3">
+      <c r="A16">
         <v>2039</v>
       </c>
-      <c r="B16" s="3">
-        <v>10987</v>
-      </c>
-      <c r="C16" s="4">
-        <v>7753684.8700000001</v>
-      </c>
-      <c r="D16" s="4">
-        <v>2109961.4700000002</v>
+      <c r="B16" s="1">
+        <v>51135</v>
+      </c>
+      <c r="C16">
+        <v>4774798.6816189298</v>
+      </c>
+      <c r="D16">
+        <v>2263948.6028744099</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="3">
+      <c r="A17">
         <v>2040</v>
       </c>
-      <c r="B17" s="3">
-        <v>11352</v>
-      </c>
-      <c r="C17" s="4">
-        <v>9820209.9600000009</v>
-      </c>
-      <c r="D17" s="4">
-        <v>2649886.13</v>
+      <c r="B17" s="1">
+        <v>51501</v>
+      </c>
+      <c r="C17">
+        <v>5750930.2479360299</v>
+      </c>
+      <c r="D17">
+        <v>2733806.52242336</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="3">
+      <c r="A18">
         <v>2041</v>
       </c>
-      <c r="B18" s="3">
-        <v>11717</v>
-      </c>
-      <c r="C18" s="4">
-        <v>12331357.57</v>
-      </c>
-      <c r="D18" s="4">
-        <v>3304142.34</v>
+      <c r="B18" s="1">
+        <v>51866</v>
+      </c>
+      <c r="C18">
+        <v>6883650.1914255004</v>
+      </c>
+      <c r="D18">
+        <v>3280418.4059483502</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="3">
+      <c r="A19">
         <v>2042</v>
       </c>
-      <c r="B19" s="3">
-        <v>12082</v>
-      </c>
-      <c r="C19" s="4">
-        <v>15367991.939999999</v>
-      </c>
-      <c r="D19" s="4">
-        <v>4093712.02</v>
+      <c r="B19" s="1">
+        <v>52231</v>
+      </c>
+      <c r="C19">
+        <v>8195384.2274682401</v>
+      </c>
+      <c r="D19">
+        <v>3914968.6236715699</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="3">
+      <c r="A20">
         <v>2043</v>
       </c>
-      <c r="B20" s="3">
-        <v>12447</v>
-      </c>
-      <c r="C20" s="4">
-        <v>18999817.309999999</v>
-      </c>
-      <c r="D20" s="4">
-        <v>5044464.6500000004</v>
+      <c r="B20" s="1">
+        <v>52596</v>
+      </c>
+      <c r="C20">
+        <v>9707887.5908375997</v>
+      </c>
+      <c r="D20">
+        <v>4648382.3099551098</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="3">
+      <c r="A21">
         <v>2044</v>
       </c>
-      <c r="B21" s="3">
-        <v>12812</v>
-      </c>
-      <c r="C21" s="4">
-        <v>23313231.18</v>
-      </c>
-      <c r="D21" s="4">
-        <v>6187501.4199999999</v>
+      <c r="B21" s="1">
+        <v>52962</v>
+      </c>
+      <c r="C21">
+        <v>11449902.892984699</v>
+      </c>
+      <c r="D21">
+        <v>5495042.2910539303</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="3">
+      <c r="A22">
         <v>2045</v>
       </c>
-      <c r="B22" s="3">
-        <v>13177</v>
-      </c>
-      <c r="C22" s="4">
-        <v>28401478.48</v>
-      </c>
-      <c r="D22" s="4">
-        <v>7558888.3399999999</v>
+      <c r="B22" s="1">
+        <v>53327</v>
+      </c>
+      <c r="C22">
+        <v>13437626.4973986</v>
+      </c>
+      <c r="D22">
+        <v>6463296.6480628503</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="3">
+      <c r="A23">
         <v>2046</v>
       </c>
-      <c r="B23" s="3">
-        <v>13542</v>
-      </c>
-      <c r="C23" s="4">
-        <v>34356517.039999999</v>
-      </c>
-      <c r="D23" s="4">
-        <v>9199175.9600000009</v>
+      <c r="B23" s="1">
+        <v>53692</v>
+      </c>
+      <c r="C23">
+        <v>15703267.564130301</v>
+      </c>
+      <c r="D23">
+        <v>7569343.0698924102</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="3">
+      <c r="A24">
         <v>2047</v>
       </c>
-      <c r="B24" s="3">
-        <v>13907</v>
-      </c>
-      <c r="C24" s="4">
-        <v>41271144.43</v>
-      </c>
-      <c r="D24" s="4">
-        <v>11158781.199999999</v>
+      <c r="B24" s="1">
+        <v>54057</v>
+      </c>
+      <c r="C24">
+        <v>18276812.193210401</v>
+      </c>
+      <c r="D24">
+        <v>8828378.05664335</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="3">
+      <c r="A25">
         <v>2048</v>
       </c>
-      <c r="B25" s="3">
-        <v>14272</v>
-      </c>
-      <c r="C25" s="4">
-        <v>49246125.009999998</v>
-      </c>
-      <c r="D25" s="4">
-        <v>13496520.92</v>
+      <c r="B25" s="1">
+        <v>54423</v>
+      </c>
+      <c r="C25">
+        <v>21199057.620427899</v>
+      </c>
+      <c r="D25">
+        <v>10260975.7073448</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="3">
+      <c r="A26">
         <v>2049</v>
       </c>
-      <c r="B26" s="3">
-        <v>14637</v>
-      </c>
-      <c r="C26" s="4">
-        <v>58380455.850000001</v>
-      </c>
-      <c r="D26" s="4">
-        <v>16281575.109999999</v>
+      <c r="B26" s="1">
+        <v>54788</v>
+      </c>
+      <c r="C26">
+        <v>24488877.740530901</v>
+      </c>
+      <c r="D26">
+        <v>11877039.5892299</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="3">
+      <c r="A27">
         <v>2050</v>
       </c>
-      <c r="B27" s="3">
-        <v>15002</v>
-      </c>
-      <c r="C27" s="4">
-        <v>68772776.530000001</v>
-      </c>
-      <c r="D27" s="4">
-        <v>19582980.07</v>
+      <c r="B27" s="1">
+        <v>55153</v>
+      </c>
+      <c r="C27">
+        <v>28191102.832252402</v>
+      </c>
+      <c r="D27">
+        <v>13699279.123971401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>